<commit_message>
fix queuepriority types conflict
</commit_message>
<xml_diff>
--- a/product/data.xlsx
+++ b/product/data.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/Desktop/BK/201/Truyền số liệu và mạng/MR_Phạm Quang Thái/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/Desktop/BK/201/Truyền số liệu và mạng/MR_Phạm Quang Thái/product/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712C3238-023B-F845-96C6-3C509A3B51F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B1BA9D-3E52-BE46-89A3-849664DFD09D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="460" windowWidth="27540" windowHeight="10900" xr2:uid="{959B7E49-FCCB-8C46-BD62-F6202D45503D}"/>
+    <workbookView xWindow="18460" yWindow="1300" windowWidth="10000" windowHeight="9440" xr2:uid="{959B7E49-FCCB-8C46-BD62-F6202D45503D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,12 +25,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Probability</t>
   </si>
   <si>
     <t>Symbol</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>K</t>
   </si>
 </sst>
 </file>
@@ -66,8 +99,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -385,16 +421,19 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="10.83203125" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -402,88 +441,88 @@
       <c r="A2">
         <v>0.21</v>
       </c>
-      <c r="B2">
-        <v>25</v>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
         <v>0.17</v>
       </c>
-      <c r="B3">
-        <v>24</v>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
         <v>0.15</v>
       </c>
-      <c r="B4">
-        <v>26</v>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
         <v>0.12</v>
       </c>
-      <c r="B5">
-        <v>23</v>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
-        <v>0.1</v>
-      </c>
-      <c r="B6">
-        <v>27</v>
+        <v>0.11</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7">
-        <v>0.06</v>
-      </c>
-      <c r="B7">
-        <v>22</v>
+        <v>0.08</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8">
-        <v>4.9000000000000002E-2</v>
-      </c>
-      <c r="B8">
-        <v>28</v>
+        <v>0.04</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9">
-        <v>5.0999999999999997E-2</v>
-      </c>
-      <c r="B9">
-        <v>21</v>
+        <v>0.04</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10">
         <v>0.04</v>
       </c>
-      <c r="B10">
-        <v>29</v>
+      <c r="B10" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11">
-        <v>0.03</v>
-      </c>
-      <c r="B11">
-        <v>20</v>
+        <v>0.02</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12">
         <v>0.02</v>
       </c>
-      <c r="B12">
-        <v>30</v>
+      <c r="B12" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
print HMTree by Tikz Latex
</commit_message>
<xml_diff>
--- a/product/data.xlsx
+++ b/product/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/Desktop/BK/201/Truyền số liệu và mạng/MR_Phạm Quang Thái/product/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B1BA9D-3E52-BE46-89A3-849664DFD09D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A86057-C955-E545-9F0D-C01BF60DE32D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18460" yWindow="1300" windowWidth="10000" windowHeight="9440" xr2:uid="{959B7E49-FCCB-8C46-BD62-F6202D45503D}"/>
+    <workbookView xWindow="22240" yWindow="1320" windowWidth="10000" windowHeight="9440" xr2:uid="{959B7E49-FCCB-8C46-BD62-F6202D45503D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -421,7 +421,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -471,7 +471,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>6</v>
@@ -479,7 +479,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7">
-        <v>0.08</v>
+        <v>0.06</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>7</v>
@@ -487,7 +487,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8">
-        <v>0.04</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>8</v>
@@ -495,7 +495,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9">
-        <v>0.04</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>9</v>
@@ -511,7 +511,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>11</v>

</xml_diff>